<commit_message>
update pin map, add RT1176 pin map
</commit_message>
<xml_diff>
--- a/RT1062_Pin_Functions.xlsx
+++ b/RT1062_Pin_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynn/Desktop/f/projects/present/adcs-hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynn/adcs-hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECA68F6-031D-0D4C-9360-6428BB1ACCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E5CA1-5DFE-FE4C-B738-52468E2361F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="2480" windowWidth="24620" windowHeight="15420" xr2:uid="{DA0D0CB3-E4DC-074D-9E72-FFB48C0340DC}"/>
+    <workbookView xWindow="12740" yWindow="3720" windowWidth="24620" windowHeight="15420" xr2:uid="{DA0D0CB3-E4DC-074D-9E72-FFB48C0340DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C84E9F7-2C99-E74C-845C-95B0F727800E}">
   <dimension ref="A1:I155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="111" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="111" workbookViewId="0">
       <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>

</xml_diff>